<commit_message>
Update Phenobottle Hardware BOM.xlsx
</commit_message>
<xml_diff>
--- a/Phenobottle Hardware BOM.xlsx
+++ b/Phenobottle Hardware BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentutsedu-my.sharepoint.com/personal/11686146_student_uts_edu_au/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\GitHub\Phenobottle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{53471C36-A8E4-4676-B7F3-21187E7AFD26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{20EDBB16-21C2-4ADD-8413-D2706A292892}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C76074-7E54-4863-B10D-DEB867EA2F0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28950" yWindow="-5145" windowWidth="14790" windowHeight="23175" xr2:uid="{F69BE1CC-620C-4E69-897A-6587C738318C}"/>
+    <workbookView xWindow="29970" yWindow="-8115" windowWidth="14775" windowHeight="15600" xr2:uid="{F69BE1CC-620C-4E69-897A-6587C738318C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="80">
   <si>
     <t>Item</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>Glued inside cap to attach silicone tubing to</t>
+  </si>
+  <si>
+    <t>Neudynium Magnets</t>
+  </si>
+  <si>
+    <t>5 mm OD x 2 mm W</t>
   </si>
 </sst>
 </file>
@@ -633,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C80D1D-790B-447C-9E17-E3097EF6D6FF}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,6 +1050,20 @@
         <v>77</v>
       </c>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1051,6 +1071,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8387031D9859940BA2CEA0556509EE9" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2313b6e41c438fc9e684cfae0bc3518f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f8a9a2b4-e8fa-4a55-a5a7-ecb03968497b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7564487bf455ed3880ac531cb510f064" ns3:_="">
     <xsd:import namespace="f8a9a2b4-e8fa-4a55-a5a7-ecb03968497b"/>
@@ -1228,22 +1263,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29B565B3-F0C6-4D1E-A53B-F63D44D1EA32}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8857E730-9FC2-4495-A686-D7E87783454B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDEC5790-53DF-444A-8A52-EF9A2B888D0E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1259,21 +1296,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8857E730-9FC2-4495-A686-D7E87783454B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29B565B3-F0C6-4D1E-A53B-F63D44D1EA32}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>